<commit_message>
API Developed with FastAPI
</commit_message>
<xml_diff>
--- a/Output/df.xlsx
+++ b/Output/df.xlsx
@@ -483,31 +483,36 @@
 Instructions for empty input:
 - If the user has no education data, return an empty string (do not generate any LaTeX).
 User input:
-Rajshahi University, Bangladesh. 2019-2014, Bsc in Engeneering, EEE, cgpa 3.76.
-Saint Joseph Higher Secondary School, Science, 16-18.
+B.Sc. in Computer Science, RUET, Bangladesh, 2024, First Class with Distinction H.S.C., Dhaka College, Bangladesh, 2020, GPA 5.00
 </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>\begin{twocolentry}{\textit{Rajshahi, Bangladesh}\\\textit{2014 – 2019}}
-        \textbf{Rajshahi University}
-        \textit{Bsc in Engeneering, EEE}
+          <t>\begin{twocolentry}{
+    \textit{Bangladesh}\\
+    \textit{2024}}
+        \textbf{RUET}
+        \textit{B.Sc. in Computer Science}
 \end{twocolentry}
 \vspace{0.10 cm}
 \begin{onecolentry}
     \begin{highlights}
-        \item \textbf{GPA/CGPA:} 3.76
+        \item \textbf{GPA/CGPA:} First Class with Distinction
     \end{highlights}
     \vspace{0.1 cm}
 \end{onecolentry}
-\begin{twocolentry}{\textit{}\\\textit{2016 – 2018}}
-        \textbf{Saint Joseph Higher Secondary School}
-        \textit{Science}
+\vspace{0.10 cm}
+\begin{twocolentry}{
+    \textit{Bangladesh}\\
+    \textit{2020}}
+        \textbf{Dhaka College}
+        \textit{H.S.C.}
 \end{twocolentry}
 \vspace{0.10 cm}
 \begin{onecolentry}
     \begin{highlights}
+        \item \textbf{GPA/CGPA:} 5.00
     \end{highlights}
     \vspace{0.1 cm}
 \end{onecolentry}</t>
@@ -517,7 +522,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>skills</t>
+          <t>experience</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -525,42 +530,59 @@
           <t xml:space="preserve">
 You are an expert LaTeX resume writer.
 STRICTLY follow these rules:
-1. ONLY return valid LaTeX code for the Skills section using RenderCV style.
-2. Do NOT include headings, comments, or extra text.
+1. ONLY return valid LaTeX code for the Experience section using RenderCV style.
+2. Do NOT include headings, titles, comments, explanations, or extra text.
 3. Output must be ready to merge directly into a LaTeX document.
-Requirements:
-- User input may be unorganized, just a list of skills separated by commas, spaces, or newlines.
-- Automatically create 1–5 relevant categories based on the input.
-- Each category should have a short title in bold.
-- Display skills in comma-separated lists under each category.
-- Use this LaTeX table format consistently:
-\\begin{minipage}{\\textwidth}
-    \\setlength{\\leftskip}{0.15in}
-    \\begin{tabular}{@{}p{3cm}p{0.5cm}p{12.5cm}@{}}
-        \\small{\\textbf{Category 1}} &amp; \\textbf{:} &amp; \\small{skills here} \\\\
-        \\small{\\textbf{Category 2}} &amp; \\textbf{:} &amp; \\small{skills here} \\\\
-        ...
-    \\end{tabular}
-\\end{minipage}
-- If the user input is empty, return an empty string.
-- Add some extra relevant skills that match the categories if applicable.
+For each experience entry, follow this exact format:
+\begin{twocolentry}{
+    \textit{&lt;City, Country&gt;}\\
+    \textit{&lt;Start Year&gt; – &lt;End Year or Present&gt;}}
+        \textbf{&lt;Company/Organization Name&gt;}
+        \textit{&lt;Job Title or Role&gt;}
+\end{twocolentry}
+\begin{onecolentry}
+    \begin{highlights}
+        \item &lt;Responsibility or Achievement 1&gt;
+        \item &lt;Responsibility or Achievement 2&gt;
+        \item &lt;Responsibility or Achievement 3&gt;
+    \end{highlights}
+    \vspace{0.1 cm}
+\end{onecolentry}
+Instructions for multiple entries:
+- Generate entries **in the order provided by the user**.
+Instructions for empty input:
+- If the user has no experience data, return an empty string (do not generate any LaTeX).
 User input:
-Matlab, Autocad, C, Arduino, Scaps1D,
-Communication skill.
-Ms word, excel.
+Software Engineer, XYZ Tech, Dhaka, 2024–Present: Developed a web app that improved user engagement by 30%. Intern, ABC Solutions, Dhaka, Summer 2023: Assisted in implementing ML-based recommendation system
 </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>\begin{minipage}{\textwidth}
-    \setlength{\leftskip}{0.15in}
-    \begin{tabular}{@{}p{3cm}p{0.5cm}p{12.5cm}@{}}
-        \small{\textbf{Programming Languages}} &amp; \textbf{:} &amp; \small{C, Matlab} \\
-        \small{\textbf{Software Tools}} &amp; \textbf{:} &amp; \small{AutoCAD, MS Word, MS Excel, Scaps1D, Arduino IDE} \\
-        \small{\textbf{Soft Skills}} &amp; \textbf{:} &amp; \small{Communication skill} \\
-    \end{tabular}
-\end{minipage}</t>
+          <t>\begin{twocolentry}{
+    \textit{Dhaka, Bangladesh}\\
+    \textit{2024 – Present}}
+        \textbf{XYZ Tech}
+        \textit{Software Engineer}
+\end{twocolentry}
+\begin{onecolentry}
+    \begin{highlights}
+        \item Developed a web app that improved user engagement by 30\%.
+    \end{highlights}
+    \vspace{0.1 cm}
+\end{onecolentry}
+\begin{twocolentry}{
+    \textit{Dhaka, Bangladesh}\\
+    \textit{Summer 2023}}
+        \textbf{ABC Solutions}
+        \textit{Intern}
+\end{twocolentry}
+\begin{onecolentry}
+    \begin{highlights}
+        \item Assisted in implementing ML-based recommendation system.
+    \end{highlights}
+    \vspace{0.1 cm}
+\end{onecolentry}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Pdf, Video added . DEMO
</commit_message>
<xml_diff>
--- a/Output/df.xlsx
+++ b/Output/df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,52 +453,10 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>thesis</t>
+          <t>education</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-You are an expert LaTeX resume writer.
-STRICTLY follow these rules:
-1. ONLY return valid LaTeX code for the Undergraduate Thesis section using RenderCV style.
-2. Do NOT include comments, explanations, or headings outside LaTeX.
-3. Output must be ready to merge directly into a LaTeX document.
-Format for the thesis entry:
-\begin{onecolentry}
-    \textbf{&lt;Thesis Title&gt;}\\
-    \small \textit{&lt;Keywords / Tools / Methods used&gt;}
-    \begin{itemize}
-    \Only One item here
-        \item &lt;Descriptive paragraph (2–3 sentences) explaining the problem, methodology, experiments, and findings. Write in professional academic tone.&gt;
-    \end{itemize}
-\end{onecolentry}
-Instructions for empty input:
-- If no undergraduate thesis is provided, return an empty string.
-User input:
-I worked on EEG signals in my thesis 2023
-</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>\begin{onecolentry}
-    \textbf{Analysis of EEG Signals}\\
-    \small \textit{EEG signal processing, Time-frequency analysis, Machine learning}
-    \begin{itemize}
-        \item This thesis investigated the characteristics of EEG signals using time-frequency analysis techniques.  Machine learning algorithms were applied to classify different brain states based on extracted features, demonstrating improved accuracy compared to existing methods. The results contribute to a better understanding of brain dynamics and potential applications in clinical diagnostics.
-    \end{itemize}
-\end{onecolentry}</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>education</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
         <is>
           <t xml:space="preserve">
 You are an expert LaTeX resume writer.
@@ -525,17 +483,45 @@
 Instructions for empty input:
 - If the user has no education data, return an empty string (do not generate any LaTeX).
 User input:
-I studied at NDC 2018
+I completed my graduation from Rajshahi University of Engineering &amp; Technology in Bsc in CSE, 2018 - 2024
+Passed HSC from Notre Dame College, 2016 - 2018 in Science Group
+Passed SSC from Brahmondi K.K.M. Govt. High School in 2014 - 2016 in Science Group
 </t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>\begin{twocolentry}{
-    \textit{}\\
-    \textit{2018 – 2018}}
-        \textbf{NDC}
-        \textit{}
+    \textit{Rajshahi, Bangladesh}\\
+    \textit{2018 – 2024}}
+        \textbf{Rajshahi University of Engineering \&amp; Technology}
+        \textit{Bsc in CSE}
+\end{twocolentry}
+\vspace{0.10 cm}
+\begin{onecolentry}
+    \begin{highlights}
+        \item \textbf{GPA/CGPA:} 
+    \end{highlights}
+    \vspace{0.1 cm}
+\end{onecolentry}
+\begin{twocolentry}{
+    \textit{Dhaka, Bangladesh}\\
+    \textit{2016 – 2018}}
+        \textbf{Notre Dame College}
+        \textit{HSC in Science Group}
+\end{twocolentry}
+\vspace{0.10 cm}
+\begin{onecolentry}
+    \begin{highlights}
+        \item \textbf{GPA/CGPA:} 
+    \end{highlights}
+    \vspace{0.1 cm}
+\end{onecolentry}
+\begin{twocolentry}{
+    \textit{Brahmondi, Bangladesh}\\
+    \textit{2014 – 2016}}
+        \textbf{Brahmondi K.K.M. Govt. High School}
+        \textit{SSC in Science Group}
 \end{twocolentry}
 \vspace{0.10 cm}
 \begin{onecolentry}
@@ -547,56 +533,243 @@
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>experience</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>thesis</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t xml:space="preserve">
 You are an expert LaTeX resume writer.
 STRICTLY follow these rules:
-1. ONLY return valid LaTeX code for the Experience section using RenderCV style.
-2. Do NOT include headings, titles, comments, explanations, or extra text.
+1. ONLY return valid LaTeX code for the Undergraduate Thesis section using RenderCV style.
+2. Do NOT include comments, explanations, or headings outside LaTeX.
 3. Output must be ready to merge directly into a LaTeX document.
-For each experience entry, follow this exact format:
-\begin{twocolentry}{
-    \textit{&lt;City, Country&gt;}\\
-    \textit{&lt;Start Year&gt; – &lt;End Year or Present&gt;}}
-        \textbf{&lt;Company/Organization Name&gt;}
-        \textit{&lt;Job Title or Role&gt;}
-\end{twocolentry}
-\begin{onecolentry}
-    \begin{highlights}
-        \item &lt;Responsibility or Achievement 1&gt;
-        \item &lt;Responsibility or Achievement 2&gt;
-        \item &lt;Responsibility or Achievement 3&gt;
-    \end{highlights}
-    \vspace{0.1 cm}
-\end{onecolentry}
-Instructions for multiple entries:
-- Generate entries **in the order provided by the user**.
+Format for the thesis entry:
+\begin{onecolentry}
+    \textbf{&lt;Thesis Title&gt;}\\
+    \small \textit{&lt;Keywords / Tools / Methods used&gt;}
+    \begin{itemize}
+    \Only One item here
+        \item &lt;Descriptive paragraph (2–3 sentences) explaining the problem, methodology, experiments, and findings. Write in professional academic tone.&gt;
+    \end{itemize}
+\end{onecolentry}
 Instructions for empty input:
-- If the user has no experience data, return an empty string (do not generate any LaTeX).
+- If no undergraduate thesis is provided, return an empty string.
 User input:
-I worked as a car mechanixs from 2999
+I conducted my thesis on Exploring EEG signals for predicting human emotions using Machine learning and Deep learning methods.
+One of my key contribution is the feature extraction techniques that I conducted in my research.
 </t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>\begin{onecolentry}
+    \textbf{Exploring EEG Signals for Predicting Human Emotions Using Machine Learning and Deep Learning Methods}\\
+    \small \textit{EEG, Machine Learning, Deep Learning, Feature Extraction}
+    \begin{itemize}
+        \item This thesis investigated the feasibility of predicting human emotions from electroencephalography (EEG) signals using machine learning and deep learning techniques.  A novel feature extraction method was developed and implemented, significantly improving the accuracy of emotion classification compared to existing approaches.  The results demonstrate the potential of this methodology for applications in affective computing and human-computer interaction.
+    \end{itemize}
+\end{onecolentry}</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>projects</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+You are an expert LaTeX resume writer.
+STRICTLY follow these rules:
+1. ONLY return valid LaTeX code for the Projects section using RenderCV style.
+2. Do NOT include headings, comments, or explanations.
+3. Output must be ready to merge directly into a LaTeX document.
+Format for each project:
+\begin{onecolentry}
+    \textbf{&lt;Project Title&gt;} \\ 
+    \small \textit{&lt;Technologies / Tools / Methods&gt;} \\
+    \small \textit{\href{&lt;URL&gt;}{Source}}  # Include this line only if a link is provided
+    \begin{itemize}
+        \item &lt;Project description / responsibility 1&gt;
+        \item &lt;Project description / responsibility 2&gt;
+    \end{itemize}
+\end{onecolentry}
+\vspace{0.1cm}
+Instructions:
+- If the project is ongoing, add "– \textit{Ongoing}" after the title.
+- Repeat the structure for multiple projects in the order provided.
+- If no projects are provided, return an empty string.
+User input:
+I have several projects.
+I made PromptFolio, which makes CV latex code usinf LLM, this is a full flex project, with frontend, Backend, and API.
+I also have made 6 bit CPU, using ADD, MUL, DIV, operation, in my computer architecture course.
+I also made a Website of my own portfolio.
+I made A sentimentFlex app, which predicts a movie;s sentiment, if it is good, or bad revied, using Naive Bayes algorithm, and NLP Techniques
+I have another project called Road pavement detection.. this is a classification project, I detected, if a road is broken or not., or it has potholes, crackes in it or not. I made this using Yolo algorithm. Created a custom dataset.
+</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>\begin{twocolentry}{
-    \textit{}\\
-    \textit{2999 – }}
-        \textbf{}
-        \textit{car mechanixs}
-\end{twocolentry}
-\begin{onecolentry}
-    \begin{highlights}
-    \end{highlights}
-    \vspace{0.1 cm}
+          <t>\begin{onecolentry}
+    \textbf{PromptFolio} \\
+    \small \textit{Frontend, Backend, API, LLM} \\
+    \begin{itemize}
+        \item Developed a full-stack application generating LaTeX CV code using Large Language Models.
+        \item Designed and implemented the frontend, backend, and API infrastructure.
+    \end{itemize}
+\end{onecolentry}
+\vspace{0.1cm}
+\begin{onecolentry}
+    \textbf{6-bit CPU} \\
+    \small \textit{Computer Architecture} \\
+    \begin{itemize}
+        \item Designed and implemented a 6-bit CPU with ADD, MUL, and DIV operations.
+        \item Completed as part of a computer architecture course.
+    \end{itemize}
+\end{onecolentry}
+\vspace{0.1cm}
+\begin{onecolentry}
+    \textbf{Personal Portfolio Website} \\
+    \small \textit{} \\
+    \begin{itemize}
+        \item Developed a personal website to showcase projects and skills.
+    \end{itemize}
+\end{onecolentry}
+\vspace{0.1cm}
+\begin{onecolentry}
+    \textbf{SentimentFlex App} \\
+    \small \textit{Naive Bayes, NLP} \\
+    \begin{itemize}
+        \item Created an application predicting movie sentiment (positive or negative reviews) using Naive Bayes algorithm and NLP techniques.
+    \end{itemize}
+\end{onecolentry}
+\vspace{0.1cm}
+\begin{onecolentry}
+    \textbf{Road Pavement Detection} \\
+    \small \textit{YOLO Algorithm, Custom Dataset} \\
+    \begin{itemize}
+        \item Developed a classification model to detect road damage (potholes, cracks) using the YOLO algorithm.
+        \item Created a custom dataset for training and evaluation.
+    \end{itemize}
+\end{onecolentry}
+\vspace{0.1cm}</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>skills</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+You are an expert LaTeX resume writer.
+STRICTLY follow these rules:
+1. ONLY return valid LaTeX code for the Skills section using RenderCV style.
+2. Do NOT include headings, comments, or extra text.
+3. Output must be ready to merge directly into a LaTeX document.
+Requirements:
+- User input may be unorganized, just a list of skills separated by commas, spaces, or newlines.
+- Automatically create 1–5 relevant categories based on the input.
+- Each category should have a short title in bold.
+- Display skills in comma-separated lists under each category.
+- Use this LaTeX table format consistently:
+\\begin{minipage}{\\textwidth}
+    \\setlength{\\leftskip}{0.15in}
+    \\begin{tabular}{@{}p{3cm}p{0.5cm}p{12.5cm}@{}}
+        \\small{\\textbf{Category 1}} &amp; \\textbf{:} &amp; \\small{skills here} \\\\
+        \\small{\\textbf{Category 2}} &amp; \\textbf{:} &amp; \\small{skills here} \\\\
+        ...
+    \\end{tabular}
+\\end{minipage}
+- If the user input is empty, return an empty string.
+- Add some extra relevant skills that match the categories if applicable.
+User input:
+I have many skills, I have communication skills,
+graphic designing,
+Computer programmings, like C, C++, Pythin, Java, etc.
+I have Data handling capabilities, I mastered in Feature extraction techniques, 
+I also have Music production skills, Fl studio, Music editing, Video making, 
+</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>\begin{minipage}{\textwidth}
+    \setlength{\leftskip}{0.15in}
+    \begin{tabular}{@{}p{3cm}p{0.5cm}p{12.5cm}@{}}
+        \small{\textbf{Programming Languages}} &amp; \textbf{:} &amp; \small{C, C++, Python, Java, JavaScript} \\
+        \small{\textbf{Data Science}} &amp; \textbf{:} &amp; \small{Data Handling, Feature Extraction, Data Analysis, Machine Learning} \\
+        \small{\textbf{Design}} &amp; \textbf{:} &amp; \small{Graphic Designing, Visual Communication,  UI/UX Design} \\
+        \small{\textbf{Audio/Video Production}} &amp; \textbf{:} &amp; \small{Music Production, Music Editing, Video Making, FL Studio, Audio Engineering} \\
+        \small{\textbf{Communication}} &amp; \textbf{:} &amp; \small{Communication Skills, Public Speaking, Technical Writing} \\
+    \end{tabular}
+\end{minipage}</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>awards</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+You are an expert LaTeX resume writer.
+STRICTLY follow these rules:
+1. ONLY return valid LaTeX code for the Leadership &amp; Awards section using RenderCV style.
+2. Do NOT include headings, comments, or extra text.
+3. Output must be ready to merge directly into a LaTeX document.
+Requirements:
+- User input may be unorganized text about leadership roles, awards, recognitions, or honors.
+- Each entry must be formatted inside a \begin{onecolentry} and \begin{highlights} block.
+- Each award or role should be a \item with:
+    • Bold title (\textbf{...})
+    • Small italic text for organization / date if needed (\small \textit{...})
+    • Description in a nested \begin{itemize} block with one or two bullet points.
+- Add \vspace{-0.1 cm} after each \item for spacing.
+- Repeat the structure for multiple entries in the order provided.
+- If no entries are provided, return an empty string.
+User input:
+I was honored by SSC, JSC, HSC scholarship by the govt of Bangladesh
+I was the vice president of RUET cultural club
+I am the lifetime member of NDCC
+</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>\begin{onecolentry}
+\begin{highlights}
+\item \textbf{SSC, JSC, HSC Scholarship} \small \textit{Government of Bangladesh}
+\begin{itemize}
+\item Awarded for academic excellence.
+\item Recognition of top performance in secondary and higher secondary education.
+\end{itemize}
+\vspace{-0.1cm}
+\item \textbf{Vice President, RUET Cultural Club} \small \textit{Rajshahi University of Engineering &amp; Technology}
+\begin{itemize}
+\item Led and managed various cultural events and initiatives.
+\item Contributed to the club's overall success and growth.
+\end{itemize}
+\vspace{-0.1cm}
+\item \textbf{Lifetime Member} \small \textit{NDCC}
+\begin{itemize}
+\item Recognition of continued commitment and support.
+\end{itemize}
+\vspace{-0.1cm}
+\end{highlights}
 \end{onecolentry}</t>
         </is>
       </c>

</xml_diff>